<commit_message>
Se genera clase Managemente para agrupar todo el proceso de lectura de archivo origen, generacion de archivo logico, guardado de archivo.
</commit_message>
<xml_diff>
--- a/Results/DEPOR_18042021.xlsx
+++ b/Results/DEPOR_18042021.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,121 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COMERCIAL DEPOR </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>UMBRO</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>64</v>
+      </c>
+      <c r="D2" t="n">
+        <v>18107028</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18107028-5</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>GARCIA</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>FUENTES</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ABNER ENRIQUE</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>41913</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PROMOTOR (A)                            </t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>MELLADO 90</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>CHIGUAYANTE</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>CHIGUAYANTE</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>ABNER ENRIQUE GARCIA FUENTES</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CONCEPCIÓN                              </t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Banco Falabella               </t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50012549283                         </t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CUENTA VISTA </t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>44260</v>
+      </c>
+      <c r="V2" t="n">
+        <v>44261</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>abgarcia2092@gmail.com</t>
+        </is>
+      </c>
+      <c r="Y2" t="n">
+        <v>10568154</v>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Suspendido</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -497,38 +612,38 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D3" t="n">
-        <v>18107028</v>
+        <v>18800233</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>18107028-5</t>
+          <t>18800233-1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>GARCIA</t>
+          <t>ESPINOZA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>FUENTES</t>
+          <t>LAGOS</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ABNER ENRIQUE</t>
+          <t>ALEXIS</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>41913</v>
+        <v>42328</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -537,27 +652,27 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>MELLADO 90</t>
+          <t>ISABEL ORTEGA 1151</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>CHIGUAYANTE</t>
+          <t xml:space="preserve">LOS ANGELES                             </t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>CHIGUAYANTE</t>
+          <t xml:space="preserve">LOS ANGELES                             </t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>ABNER ENRIQUE GARCIA FUENTES</t>
+          <t>ALEXIS ESPINOZA LAGOS</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t xml:space="preserve">CONCEPCIÓN                              </t>
+          <t xml:space="preserve">LOS ÁNGELES                             </t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -572,7 +687,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t xml:space="preserve">50012549283                         </t>
+          <t xml:space="preserve">50013491675                         </t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -580,136 +695,21 @@
           <t xml:space="preserve">CUENTA VISTA </t>
         </is>
       </c>
-      <c r="U3" t="n">
-        <v>44260</v>
-      </c>
       <c r="V3" t="n">
-        <v>44261</v>
+        <v>44247</v>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>abgarcia2092@gmail.com</t>
-        </is>
+          <t>alexislake26@gmail.com</t>
+        </is>
+      </c>
+      <c r="X3" t="n">
+        <v>974048940</v>
       </c>
       <c r="Y3" t="n">
-        <v>10568154</v>
+        <v>10496521</v>
       </c>
       <c r="Z3" t="inlineStr">
-        <is>
-          <t>Suspendido</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">COMERCIAL DEPOR </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>UMBRO</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>50</v>
-      </c>
-      <c r="D4" t="n">
-        <v>18800233</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>18800233-1</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>ESPINOZA</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>LAGOS</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>ALEXIS</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>42328</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PROMOTOR (A)                            </t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>ISABEL ORTEGA 1151</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOS ANGELES                             </t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOS ANGELES                             </t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>ALEXIS ESPINOZA LAGOS</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LOS ÁNGELES                             </t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Banco Falabella               </t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">50013491675                         </t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CUENTA VISTA </t>
-        </is>
-      </c>
-      <c r="V4" t="n">
-        <v>44247</v>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>alexislake26@gmail.com</t>
-        </is>
-      </c>
-      <c r="X4" t="n">
-        <v>974048940</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>10496521</v>
-      </c>
-      <c r="Z4" t="inlineStr">
         <is>
           <t>Suspendido</t>
         </is>

</xml_diff>